<commit_message>
Better modularisation &  avoiding hours duplicates
</commit_message>
<xml_diff>
--- a/admin/Users.xlsx
+++ b/admin/Users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/and/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/pwa-survey/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B7B021-4CFD-5344-A7A9-DAC9108DC14B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415B22A9-F695-9B43-B273-B25FE152F7E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2100" windowWidth="28040" windowHeight="17040" xr2:uid="{1F4F044D-DF06-E545-A2E6-33EF306AC5F5}"/>
+    <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{1F4F044D-DF06-E545-A2E6-33EF306AC5F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Séli</t>
   </si>
   <si>
-    <t xml:space="preserve"> Léodagan</t>
-  </si>
-  <si>
     <t>La Dame</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">roi de Calédonie </t>
+  </si>
+  <si>
+    <t>Léodagan</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,12 +541,12 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -554,58 +554,58 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Offline app fidex & CRUD activities in PWA
</commit_message>
<xml_diff>
--- a/admin/Users.xlsx
+++ b/admin/Users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/pwa-survey/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415B22A9-F695-9B43-B273-B25FE152F7E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D4552-1D4D-A342-BA87-3879001034F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{1F4F044D-DF06-E545-A2E6-33EF306AC5F5}"/>
   </bookViews>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6220FB-A815-E646-9FAD-3145FD62827C}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C15" sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,124 +488,169 @@
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>